<commit_message>
tested the code @Lo, the next step is the txt output
</commit_message>
<xml_diff>
--- a/value_messages_excel.xlsx
+++ b/value_messages_excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Lombardi_Ing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k.mosleh\MyRepos\Excel_manip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EA3075-7E19-420D-818D-E1E71979EA5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170B902A-C2A3-4790-A376-90E9E656DA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3576" yWindow="1200" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -395,8 +395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -545,13 +545,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A19" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
added the functionality to write a simple  txt/ids with the messages
</commit_message>
<xml_diff>
--- a/value_messages_excel.xlsx
+++ b/value_messages_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k.mosleh\MyRepos\Excel_manip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170B902A-C2A3-4790-A376-90E9E656DA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052F21B7-2409-4D7A-82E5-E1A45B686497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16404" windowHeight="9264" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -545,13 +545,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
keeping first and last part and modifying only the middle
</commit_message>
<xml_diff>
--- a/value_messages_excel.xlsx
+++ b/value_messages_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k.mosleh\MyRepos\Excel_manip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052F21B7-2409-4D7A-82E5-E1A45B686497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56207AF-0DF0-417F-8039-B9FA71E83D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16404" windowHeight="9264" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -395,8 +395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -545,13 +545,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.77734375" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
added indent for text base file
</commit_message>
<xml_diff>
--- a/value_messages_excel.xlsx
+++ b/value_messages_excel.xlsx
@@ -1,77 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k.mosleh\MyRepos\Excel_manip\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56207AF-0DF0-417F-8039-B9FA71E83D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Input" sheetId="1" r:id="rId1"/>
-    <sheet name="Output" sheetId="2" r:id="rId2"/>
+    <sheet name="Input" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Output" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>Row1</t>
-  </si>
-  <si>
-    <t>Row2</t>
-  </si>
-  <si>
-    <t>Row3</t>
-  </si>
-  <si>
-    <t>Row4</t>
-  </si>
-  <si>
-    <t>Row5</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -90,21 +47,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -392,147 +408,173 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
+    <row r="1">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Row1</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>10</v>
+      </c>
+      <c r="C2" t="n">
+        <v>20</v>
+      </c>
+      <c r="D2" t="n">
+        <v>30</v>
+      </c>
+      <c r="E2" t="n">
+        <v>40</v>
+      </c>
+      <c r="F2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G2" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Row2</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C3" t="n">
+        <v>25</v>
+      </c>
+      <c r="D3" t="n">
+        <v>35</v>
+      </c>
+      <c r="E3" t="n">
+        <v>45</v>
+      </c>
+      <c r="F3" t="n">
+        <v>55</v>
+      </c>
+      <c r="G3" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Row3</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
+      <c r="C4" t="n">
         <v>10</v>
       </c>
-      <c r="C2">
+      <c r="D4" t="n">
+        <v>15</v>
+      </c>
+      <c r="E4" t="n">
         <v>20</v>
       </c>
-      <c r="D2">
+      <c r="F4" t="n">
+        <v>25</v>
+      </c>
+      <c r="G4" t="n">
         <v>30</v>
       </c>
-      <c r="E2">
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Row4</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>30</v>
+      </c>
+      <c r="C5" t="n">
+        <v>35</v>
+      </c>
+      <c r="D5" t="n">
         <v>40</v>
       </c>
-      <c r="F2">
+      <c r="E5" t="n">
+        <v>45</v>
+      </c>
+      <c r="F5" t="n">
         <v>50</v>
       </c>
-      <c r="G2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>15</v>
-      </c>
-      <c r="C3">
-        <v>25</v>
-      </c>
-      <c r="D3">
-        <v>35</v>
-      </c>
-      <c r="E3">
-        <v>45</v>
-      </c>
-      <c r="F3">
+      <c r="G5" t="n">
         <v>55</v>
       </c>
-      <c r="G3">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>15</v>
-      </c>
-      <c r="E4">
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Row5</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>12</v>
+      </c>
+      <c r="C6" t="n">
+        <v>14</v>
+      </c>
+      <c r="D6" t="n">
+        <v>16</v>
+      </c>
+      <c r="E6" t="n">
+        <v>18</v>
+      </c>
+      <c r="F6" t="n">
         <v>20</v>
       </c>
-      <c r="F4">
-        <v>25</v>
-      </c>
-      <c r="G4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>30</v>
-      </c>
-      <c r="C5">
-        <v>35</v>
-      </c>
-      <c r="D5">
-        <v>40</v>
-      </c>
-      <c r="E5">
-        <v>45</v>
-      </c>
-      <c r="F5">
-        <v>50</v>
-      </c>
-      <c r="G5">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>12</v>
-      </c>
-      <c r="C6">
-        <v>14</v>
-      </c>
-      <c r="D6">
-        <v>16</v>
-      </c>
-      <c r="E6">
-        <v>18</v>
-      </c>
-      <c r="F6">
-        <v>20</v>
-      </c>
-      <c r="G6">
+      <c r="G6" t="n">
         <v>22</v>
       </c>
     </row>
@@ -542,18 +584,233 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="25.77734375" customWidth="1"/>
+    <col width="25.77734375" customWidth="1" min="1" max="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>The value from row: Row1, and column: A, is: 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>The value from row: Row1, and column: B, is: 20</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>The value from row: Row1, and column: C, is: 30</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>The value from row: Row1, and column: D, is: 40</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>The value from row: Row1, and column: E, is: 50</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>The value from row: Row1, and column: F, is: 60</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>The value from row: Row2, and column: A, is: 15</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>The value from row: Row2, and column: B, is: 25</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>The value from row: Row2, and column: C, is: 35</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>The value from row: Row2, and column: D, is: 45</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>The value from row: Row2, and column: E, is: 55</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>The value from row: Row2, and column: F, is: 65</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>The value from row: Row3, and column: A, is: 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>The value from row: Row3, and column: B, is: 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>The value from row: Row3, and column: C, is: 15</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>The value from row: Row3, and column: D, is: 20</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>The value from row: Row3, and column: E, is: 25</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>The value from row: Row3, and column: F, is: 30</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>The value from row: Row4, and column: A, is: 30</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>The value from row: Row4, and column: B, is: 35</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>The value from row: Row4, and column: C, is: 40</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>The value from row: Row4, and column: D, is: 45</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>The value from row: Row4, and column: E, is: 50</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>The value from row: Row4, and column: F, is: 55</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>The value from row: Row5, and column: A, is: 12</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>The value from row: Row5, and column: B, is: 14</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>The value from row: Row5, and column: C, is: 16</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>The value from row: Row5, and column: D, is: 18</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>The value from row: Row5, and column: E, is: 20</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>The value from row: Row5, and column: F, is: 22</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>